<commit_message>
Timing need to be fixed
</commit_message>
<xml_diff>
--- a/Horas.xlsx
+++ b/Horas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
   <si>
     <t>Atención temprana</t>
   </si>
@@ -79,21 +79,9 @@
     <t>Laia González</t>
   </si>
   <si>
-    <t>Martín</t>
-  </si>
-  <si>
     <t>Luisito cara pito</t>
   </si>
   <si>
-    <t>Miguel</t>
-  </si>
-  <si>
-    <t>Miguel Lolo</t>
-  </si>
-  <si>
-    <t>Raul</t>
-  </si>
-  <si>
     <t>Victor</t>
   </si>
   <si>
@@ -124,7 +112,7 @@
     <t>2023-01-13 --&gt; 15:00</t>
   </si>
   <si>
-    <t>2023-01-12 --&gt; 0:00</t>
+    <t>2023-01-12 --&gt; 12:30</t>
   </si>
   <si>
     <t>2023-01-06 --&gt; 12:00</t>
@@ -137,6 +125,9 @@
   </si>
   <si>
     <t>Coordinación para hablar del tiempo</t>
+  </si>
+  <si>
+    <t>asdfasd</t>
   </si>
 </sst>
 </file>
@@ -483,13 +474,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T71"/>
+  <dimension ref="A1:AA71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:27">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -518,129 +509,118 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:27">
       <c r="A2" t="s">
         <v>20</v>
       </c>
       <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2">
+        <v>26</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>27</v>
+      </c>
+      <c r="R2" t="s">
         <v>28</v>
       </c>
-      <c r="C2" t="s">
+      <c r="S2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T2" t="s">
         <v>28</v>
       </c>
-      <c r="D2" t="s">
+      <c r="U2" t="s">
+        <v>29</v>
+      </c>
+      <c r="V2" t="s">
         <v>28</v>
       </c>
-      <c r="E2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2">
-        <v>19</v>
-      </c>
-      <c r="H2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" t="s">
-        <v>29</v>
-      </c>
-      <c r="L2" t="s">
-        <v>30</v>
-      </c>
-      <c r="M2" t="s">
-        <v>30</v>
-      </c>
-      <c r="N2" t="s">
-        <v>31</v>
-      </c>
-      <c r="O2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P2" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>31</v>
-      </c>
-      <c r="R2" t="s">
-        <v>32</v>
-      </c>
-      <c r="S2" t="s">
-        <v>33</v>
-      </c>
-      <c r="T2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20">
+      <c r="W2" t="s">
+        <v>24</v>
+      </c>
+      <c r="X2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27">
       <c r="A3" t="s">
         <v>21</v>
       </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
       <c r="G3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27">
       <c r="A4" t="s">
         <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5">
         <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20">
-      <c r="A6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20">
-      <c r="A7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20">
-      <c r="A8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -648,7 +628,7 @@
         <v>12</v>
       </c>
       <c r="G38" s="1">
-        <f>SUMA(G2:G36)</f>
+        <f>SUMA(G2:G37)</f>
         <v>0</v>
       </c>
     </row>
@@ -692,13 +672,13 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B42" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C42" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G42">
         <v>2</v>
@@ -709,7 +689,7 @@
         <v>14</v>
       </c>
       <c r="G53" s="1">
-        <f>SUMA(G40:G51)</f>
+        <f>SUMA(G42:G52)</f>
         <v>0</v>
       </c>
     </row>
@@ -759,7 +739,7 @@
     </row>
     <row r="62" spans="1:7">
       <c r="A62" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B62">
         <v>36.28</v>
@@ -767,7 +747,7 @@
     </row>
     <row r="63" spans="1:7">
       <c r="A63" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B63">
         <v>36.28</v>
@@ -775,9 +755,17 @@
     </row>
     <row r="64" spans="1:7">
       <c r="A64" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B64">
+        <v>36.28</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
+        <v>37</v>
+      </c>
+      <c r="B65">
         <v>36.28</v>
       </c>
     </row>

</xml_diff>